<commit_message>
Dergi makalesi için experimental result source dosyaları. fig dosyaları büyük boyutlu olduğu için driveda bi yere koydum. @ozank, @furkankarakaya.
</commit_message>
<xml_diff>
--- a/Prototype/Test/test diaries/2019.05.05/05.05.2019 - Exp Result.xlsx
+++ b/Prototype/Test/test diaries/2019.05.05/05.05.2019 - Exp Result.xlsx
@@ -414,7 +414,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="175462864"/>
@@ -473,7 +473,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="177578384"/>
@@ -514,7 +514,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -566,7 +566,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -724,7 +724,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="304064704"/>
@@ -786,7 +786,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="304064144"/>
@@ -827,7 +827,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1128,7 +1128,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="270604752"/>
@@ -1185,7 +1185,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="304859728"/>
@@ -1226,7 +1226,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3297,7 +3297,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>